<commit_message>
Fix sample submission test
I did the easy way and removed calculation from submission file
</commit_message>
<xml_diff>
--- a/tests/fixtures/samples/gemstones-samplesubmission-unique-samples.xlsx
+++ b/tests/fixtures/samples/gemstones-samplesubmission-unique-samples.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t xml:space="preserve">PI</t>
   </si>
@@ -59,6 +59,9 @@
     <t xml:space="preserve">SAMPLE TYPE</t>
   </si>
   <si>
+    <t xml:space="preserve">sample-Frink-1693_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">A:1</t>
   </si>
   <si>
@@ -74,6 +77,9 @@
     <t xml:space="preserve">GemstoneSample</t>
   </si>
   <si>
+    <t xml:space="preserve">sample-Frink-1693_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">B:1</t>
   </si>
   <si>
@@ -81,6 +87,9 @@
   </si>
   <si>
     <t xml:space="preserve">green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample-Frink-1693_3</t>
   </si>
   <si>
     <t xml:space="preserve">C:1</t>
@@ -332,8 +341,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.34"/>
   </cols>
   <sheetData>
@@ -372,13 +381,13 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="26.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="40.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.34"/>
@@ -434,24 +443,23 @@
         <f aca="false">CONCATENATE("plate-",General!$B$1,"-",General!$B$2)</f>
         <v>plate-Frink-1693</v>
       </c>
-      <c r="B4" s="7" t="str">
-        <f aca="false">CONCATENATE("sample-",General!$B$1,"-",General!$B$2) &amp; "_1"</f>
-        <v>sample-Frink-1693_1</v>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,24 +467,23 @@
         <f aca="false">CONCATENATE("plate-",General!$B$1,"-",General!$B$2)</f>
         <v>plate-Frink-1693</v>
       </c>
-      <c r="B5" s="7" t="str">
-        <f aca="false">CONCATENATE("sample-",General!$B$1,"-",General!$B$2) &amp; "_2"</f>
-        <v>sample-Frink-1693_2</v>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -484,24 +491,23 @@
         <f aca="false">CONCATENATE("plate-",General!$B$1,"-",General!$B$2)</f>
         <v>plate-Frink-1693</v>
       </c>
-      <c r="B6" s="7" t="str">
-        <f aca="false">CONCATENATE("sample-",General!$B$1,"-",General!$B$2) &amp; "_3"</f>
-        <v>sample-Frink-1693_3</v>
+      <c r="B6" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>